<commit_message>
Major changes to the report, created a possible cover page, changed the order of some of the methods in CargoSpace and Package
</commit_message>
<xml_diff>
--- a/Report, presentation and related stuff/Experiment Data 2.xlsx
+++ b/Report, presentation and related stuff/Experiment Data 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\Documents\GitHub\PP3\Genetic Algorithm Autom Pack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\Documents\GitHub\PP3\Report, presentation and related stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="73">
   <si>
     <t>All experiments run on an i5-4790k 3.5 GHz processor</t>
   </si>
@@ -175,6 +175,75 @@
   <si>
     <t>infinite</t>
   </si>
+  <si>
+    <t>Defining properties</t>
+  </si>
+  <si>
+    <t>A, B, C + 1 similar (inf)</t>
+  </si>
+  <si>
+    <t>A, B, C + 2 similar (inf)</t>
+  </si>
+  <si>
+    <t>A, B, C + 3 similar (inf)</t>
+  </si>
+  <si>
+    <t>Small packages (inf)</t>
+  </si>
+  <si>
+    <t>Big packages (inf)</t>
+  </si>
+  <si>
+    <t>Cubes (inf)</t>
+  </si>
+  <si>
+    <t>Long packages (inf)</t>
+  </si>
+  <si>
+    <t>Flat packages (inf)</t>
+  </si>
+  <si>
+    <t>A, B, C + 1 similar (15)</t>
+  </si>
+  <si>
+    <t>A, B, C + 2 similar (15)</t>
+  </si>
+  <si>
+    <t>A, B, C + 3 similar (10)</t>
+  </si>
+  <si>
+    <t>1x1x1 (330), 0.5x1x1.5 (220), 1x1x1 (165)</t>
+  </si>
+  <si>
+    <t>2x3x3 (10), 2x2.5x3 (11), 2.5x2.5x2.5 (11)</t>
+  </si>
+  <si>
+    <t>2.5x0.5x0.5 (264), 3x1x1 (55), 4x1x0.5 (83)</t>
+  </si>
+  <si>
+    <t>1x1x1 (165), 1.5x1.5x1.5 (50), 2x2x2 (21)</t>
+  </si>
+  <si>
+    <t>2x2.5x0.5 (66), 1.5x1.5x0.5 (147), 3x2x1 (28)</t>
+  </si>
+  <si>
+    <t>A (15), B (15), C (15), 2.x2.05 (15)</t>
+  </si>
+  <si>
+    <t>A (15), B (15), C (15), 2.x2.05 (15), 3x1x1 (15)</t>
+  </si>
+  <si>
+    <t>A (10), B (10), C (10), 2.x2.05 (10), 3x1x1 (10), 2.5x1x1.5 (10)</t>
+  </si>
+  <si>
+    <t>A (83), B (55), C (50), 2.x2.05 (83)</t>
+  </si>
+  <si>
+    <t>A (83), B (55), C (50), 2.x2.05 (83), 3x1x1 (55)</t>
+  </si>
+  <si>
+    <t>A (83), B (55), C (50), 2.x2.05 (83), 3x1x1 (55), 2.5x1x1.5 (44)</t>
+  </si>
 </sst>
 </file>
 
@@ -232,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -423,11 +492,161 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -504,18 +723,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,6 +883,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -811,8 +1111,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1990374112"/>
-        <c:axId val="1990365952"/>
+        <c:axId val="2061721616"/>
+        <c:axId val="2061728688"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -917,11 +1217,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1990371936"/>
-        <c:axId val="1990378464"/>
+        <c:axId val="2061718896"/>
+        <c:axId val="2061729232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1990374112"/>
+        <c:axId val="2061721616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,6 +1267,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1033,12 +1334,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990365952"/>
+        <c:crossAx val="2061728688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990365952"/>
+        <c:axId val="2061728688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,6 +1385,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1150,12 +1452,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990374112"/>
+        <c:crossAx val="2061721616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990378464"/>
+        <c:axId val="2061729232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,6 +1489,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1252,12 +1555,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990371936"/>
+        <c:crossAx val="2061718896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990371936"/>
+        <c:axId val="2061718896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1267,7 +1570,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1990378464"/>
+        <c:crossAx val="2061729232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1281,6 +1584,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1390,6 +1694,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1605,8 +1910,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1990372480"/>
-        <c:axId val="1990369216"/>
+        <c:axId val="2061725424"/>
+        <c:axId val="2061730320"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1791,11 +2096,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1990363776"/>
-        <c:axId val="1990369760"/>
+        <c:axId val="2061728144"/>
+        <c:axId val="2061725968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1990372480"/>
+        <c:axId val="2061725424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,6 +2146,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1907,12 +2213,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990369216"/>
+        <c:crossAx val="2061730320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990369216"/>
+        <c:axId val="2061730320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,6 +2265,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2016,12 +2323,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990372480"/>
+        <c:crossAx val="2061725424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990369760"/>
+        <c:axId val="2061725968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2057,6 +2364,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2117,12 +2425,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990363776"/>
+        <c:crossAx val="2061728144"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990363776"/>
+        <c:axId val="2061728144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,7 +2440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1990369760"/>
+        <c:crossAx val="2061725968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2146,6 +2454,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2260,6 +2569,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2561,8 +2871,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1990366496"/>
-        <c:axId val="1990373024"/>
+        <c:axId val="2061726512"/>
+        <c:axId val="2061727056"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2833,11 +3143,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1990376832"/>
-        <c:axId val="1990374656"/>
+        <c:axId val="2061729776"/>
+        <c:axId val="2061727600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1990366496"/>
+        <c:axId val="2061726512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2883,6 +3193,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2949,12 +3260,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990373024"/>
+        <c:crossAx val="2061727056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990373024"/>
+        <c:axId val="2061727056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3001,6 +3312,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3058,12 +3370,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990366496"/>
+        <c:crossAx val="2061726512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990374656"/>
+        <c:axId val="2061727600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3112,6 +3424,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3172,12 +3485,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1990376832"/>
+        <c:crossAx val="2061729776"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1990376832"/>
+        <c:axId val="2061729776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3187,7 +3500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1990374656"/>
+        <c:crossAx val="2061727600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3201,6 +3514,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3310,6 +3624,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3611,8 +3926,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934545280"/>
-        <c:axId val="1934546912"/>
+        <c:axId val="2056887520"/>
+        <c:axId val="2056890784"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3883,11 +4198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934547456"/>
-        <c:axId val="1934538208"/>
+        <c:axId val="2056881536"/>
+        <c:axId val="2056880992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1934545280"/>
+        <c:axId val="2056887520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3938,6 +4253,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4004,12 +4320,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934546912"/>
+        <c:crossAx val="2056890784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934546912"/>
+        <c:axId val="2056890784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4056,6 +4372,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4113,12 +4430,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934545280"/>
+        <c:crossAx val="2056887520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934538208"/>
+        <c:axId val="2056880992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4154,6 +4471,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4214,12 +4532,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934547456"/>
+        <c:crossAx val="2056881536"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934547456"/>
+        <c:axId val="2056881536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4229,7 +4547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1934538208"/>
+        <c:crossAx val="2056880992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4243,6 +4561,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4357,6 +4676,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4640,8 +4960,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934550720"/>
-        <c:axId val="1934536576"/>
+        <c:axId val="2056886976"/>
+        <c:axId val="2056891328"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4894,11 +5214,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934538752"/>
-        <c:axId val="1934535488"/>
+        <c:axId val="2056884800"/>
+        <c:axId val="2056877184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1934550720"/>
+        <c:axId val="2056886976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4949,6 +5269,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5015,12 +5336,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934536576"/>
+        <c:crossAx val="2056891328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934536576"/>
+        <c:axId val="2056891328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5067,6 +5388,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5124,12 +5446,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934550720"/>
+        <c:crossAx val="2056886976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934535488"/>
+        <c:axId val="2056877184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5166,12 +5488,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934538752"/>
+        <c:crossAx val="2056884800"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934538752"/>
+        <c:axId val="2056884800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5181,7 +5503,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1934535488"/>
+        <c:crossAx val="2056877184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5195,6 +5517,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5304,6 +5627,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5623,8 +5947,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934537120"/>
-        <c:axId val="1934539296"/>
+        <c:axId val="2056877728"/>
+        <c:axId val="2056888064"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5913,11 +6237,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934541472"/>
-        <c:axId val="1934539840"/>
+        <c:axId val="2056879360"/>
+        <c:axId val="2056878816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1934537120"/>
+        <c:axId val="2056877728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5963,6 +6287,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6029,12 +6354,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934539296"/>
+        <c:crossAx val="2056888064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934539296"/>
+        <c:axId val="2056888064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6081,6 +6406,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6138,12 +6464,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934537120"/>
+        <c:crossAx val="2056877728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934539840"/>
+        <c:axId val="2056878816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6189,6 +6515,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6246,12 +6573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934541472"/>
+        <c:crossAx val="2056879360"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934541472"/>
+        <c:axId val="2056879360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6261,7 +6588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1934539840"/>
+        <c:crossAx val="2056878816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6275,6 +6602,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10128,10 +10456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD187"/>
+  <dimension ref="A1:AO187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL7" sqref="AL7:AO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10156,9 +10484,17 @@
     <col min="21" max="21" width="11.5703125" customWidth="1"/>
     <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
+    <col min="31" max="31" width="22.42578125" customWidth="1"/>
+    <col min="32" max="32" width="10.28515625" customWidth="1"/>
+    <col min="36" max="36" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" customWidth="1"/>
+    <col min="38" max="38" width="4.42578125" customWidth="1"/>
+    <col min="39" max="39" width="0.85546875" customWidth="1"/>
+    <col min="40" max="40" width="1" customWidth="1"/>
+    <col min="41" max="41" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10166,32 +10502,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -10219,23 +10555,49 @@
       <c r="W7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Y7" s="3" t="s">
+      <c r="Y7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Z7" s="28" t="s">
+      <c r="Z7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AA7" s="28" t="s">
+      <c r="AA7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="AB7" s="28" t="s">
+      <c r="AB7" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="AC7" s="28" t="s">
+      <c r="AC7" s="27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE7" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH7" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI7" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL7" s="53">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="54"/>
+      <c r="AN7" s="55"/>
+      <c r="AO7" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -10303,24 +10665,51 @@
       <c r="X8" t="s">
         <v>39</v>
       </c>
-      <c r="Y8" s="4">
+      <c r="Y8" s="24">
         <v>1</v>
       </c>
-      <c r="Z8" s="3">
+      <c r="Z8" s="31">
         <v>289.26</v>
       </c>
-      <c r="AA8" s="30">
+      <c r="AA8" s="32">
         <v>12479.16</v>
       </c>
-      <c r="AB8" s="3">
+      <c r="AB8" s="31">
         <v>50</v>
       </c>
-      <c r="AC8" s="29">
+      <c r="AC8" s="33">
         <f>Z8/330</f>
         <v>0.87654545454545452</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE8" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF8" s="31">
+        <v>289.26</v>
+      </c>
+      <c r="AG8" s="32">
+        <v>12479.16</v>
+      </c>
+      <c r="AH8" s="31">
+        <v>50</v>
+      </c>
+      <c r="AI8" s="47">
+        <f>AF8/330</f>
+        <v>0.87654545454545452</v>
+      </c>
+      <c r="AJ8" s="48">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="57">
+        <v>2</v>
+      </c>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="51"/>
+      <c r="AO8" s="58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>10</v>
       </c>
@@ -10388,24 +10777,51 @@
       <c r="X9" t="s">
         <v>40</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="22">
         <v>2</v>
       </c>
-      <c r="Z9" s="3">
+      <c r="Z9" s="34">
         <v>10</v>
       </c>
-      <c r="AA9" s="30">
+      <c r="AA9" s="35">
         <v>61883.96</v>
       </c>
-      <c r="AB9" s="3">
+      <c r="AB9" s="34">
         <v>123</v>
       </c>
-      <c r="AC9" s="29">
+      <c r="AC9" s="36">
         <f>Z9/11</f>
         <v>0.90909090909090906</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE9" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF9" s="34">
+        <v>10</v>
+      </c>
+      <c r="AG9" s="35">
+        <v>61883.96</v>
+      </c>
+      <c r="AH9" s="34">
+        <v>123</v>
+      </c>
+      <c r="AI9" s="39">
+        <f>AF9/11</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="AJ9" s="41">
+        <v>2</v>
+      </c>
+      <c r="AL9" s="57">
+        <v>3</v>
+      </c>
+      <c r="AM9" s="52"/>
+      <c r="AN9" s="51"/>
+      <c r="AO9" s="58" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -10473,24 +10889,51 @@
       <c r="X10" t="s">
         <v>41</v>
       </c>
-      <c r="Y10" s="4">
+      <c r="Y10" s="22">
         <v>3</v>
       </c>
-      <c r="Z10" s="3">
+      <c r="Z10" s="34">
         <v>108.56</v>
       </c>
-      <c r="AA10" s="30">
+      <c r="AA10" s="35">
         <v>45626.04</v>
       </c>
-      <c r="AB10" s="30">
+      <c r="AB10" s="35">
         <v>116</v>
       </c>
-      <c r="AC10" s="29">
+      <c r="AC10" s="36">
         <f>Z10/165</f>
         <v>0.65793939393939394</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE10" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF10" s="34">
+        <v>108.56</v>
+      </c>
+      <c r="AG10" s="35">
+        <v>45626.04</v>
+      </c>
+      <c r="AH10" s="35">
+        <v>116</v>
+      </c>
+      <c r="AI10" s="39">
+        <f>AF10/165</f>
+        <v>0.65793939393939394</v>
+      </c>
+      <c r="AJ10" s="41">
+        <v>3</v>
+      </c>
+      <c r="AL10" s="57">
+        <v>4</v>
+      </c>
+      <c r="AM10" s="52"/>
+      <c r="AN10" s="51"/>
+      <c r="AO10" s="58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>35</v>
       </c>
@@ -10558,24 +11001,51 @@
       <c r="X11" t="s">
         <v>42</v>
       </c>
-      <c r="Y11" s="4">
+      <c r="Y11" s="22">
         <v>4</v>
       </c>
-      <c r="Z11" s="3">
+      <c r="Z11" s="34">
         <v>248.6</v>
       </c>
-      <c r="AA11" s="30">
+      <c r="AA11" s="35">
         <v>85670.68</v>
       </c>
-      <c r="AB11" s="30">
+      <c r="AB11" s="35">
         <v>29.72</v>
       </c>
-      <c r="AC11" s="29">
+      <c r="AC11" s="36">
         <f>Z11/264</f>
         <v>0.94166666666666665</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE11" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF11" s="34">
+        <v>248.6</v>
+      </c>
+      <c r="AG11" s="35">
+        <v>85670.68</v>
+      </c>
+      <c r="AH11" s="35">
+        <v>29.72</v>
+      </c>
+      <c r="AI11" s="39">
+        <f>AF11/264</f>
+        <v>0.94166666666666665</v>
+      </c>
+      <c r="AJ11" s="41">
+        <v>4</v>
+      </c>
+      <c r="AL11" s="57">
+        <v>5</v>
+      </c>
+      <c r="AM11" s="52"/>
+      <c r="AN11" s="51"/>
+      <c r="AO11" s="58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>50</v>
       </c>
@@ -10643,24 +11113,51 @@
       <c r="X12" t="s">
         <v>43</v>
       </c>
-      <c r="Y12" s="4">
+      <c r="Y12" s="22">
         <v>5</v>
       </c>
-      <c r="Z12" s="3">
+      <c r="Z12" s="34">
         <v>130.68</v>
       </c>
-      <c r="AA12" s="30">
+      <c r="AA12" s="35">
         <v>81555.08</v>
       </c>
-      <c r="AB12" s="30">
+      <c r="AB12" s="35">
         <v>121.44</v>
       </c>
-      <c r="AC12" s="29">
+      <c r="AC12" s="36">
         <f>Z12/146</f>
         <v>0.89506849315068493</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE12" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF12" s="34">
+        <v>130.68</v>
+      </c>
+      <c r="AG12" s="35">
+        <v>81555.08</v>
+      </c>
+      <c r="AH12" s="35">
+        <v>121.44</v>
+      </c>
+      <c r="AI12" s="39">
+        <f>AF12/146</f>
+        <v>0.89506849315068493</v>
+      </c>
+      <c r="AJ12" s="41">
+        <v>5</v>
+      </c>
+      <c r="AL12" s="57">
+        <v>6</v>
+      </c>
+      <c r="AM12" s="52"/>
+      <c r="AN12" s="51"/>
+      <c r="AO12" s="58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>70</v>
       </c>
@@ -10728,27 +11225,54 @@
       <c r="X13" t="s">
         <v>44</v>
       </c>
-      <c r="Y13" s="4">
+      <c r="Y13" s="22">
         <v>6</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13" s="34">
         <v>186.24</v>
       </c>
-      <c r="AA13" s="30">
+      <c r="AA13" s="35">
         <v>33130.76</v>
       </c>
-      <c r="AB13" s="30">
+      <c r="AB13" s="35">
         <v>165.52</v>
       </c>
-      <c r="AC13" s="29">
+      <c r="AC13" s="36">
         <f>Z13/195</f>
         <v>0.95507692307692316</v>
       </c>
       <c r="AD13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE13" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF13" s="34">
+        <v>186.24</v>
+      </c>
+      <c r="AG13" s="35">
+        <v>33130.76</v>
+      </c>
+      <c r="AH13" s="35">
+        <v>165.52</v>
+      </c>
+      <c r="AI13" s="39">
+        <f>AF13/195</f>
+        <v>0.95507692307692316</v>
+      </c>
+      <c r="AJ13" s="41">
+        <v>6</v>
+      </c>
+      <c r="AL13" s="57">
+        <v>7</v>
+      </c>
+      <c r="AM13" s="52"/>
+      <c r="AN13" s="51"/>
+      <c r="AO13" s="58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>85</v>
       </c>
@@ -10816,27 +11340,54 @@
       <c r="X14" t="s">
         <v>45</v>
       </c>
-      <c r="Y14" s="4">
+      <c r="Y14" s="22">
         <v>7</v>
       </c>
-      <c r="Z14" s="3">
+      <c r="Z14" s="34">
         <v>187.6</v>
       </c>
-      <c r="AA14" s="3">
+      <c r="AA14" s="34">
         <v>39986.68</v>
       </c>
-      <c r="AB14" s="3">
+      <c r="AB14" s="34">
         <v>163.80000000000001</v>
       </c>
-      <c r="AC14" s="29">
+      <c r="AC14" s="36">
         <f>Z14/198</f>
         <v>0.94747474747474747</v>
       </c>
       <c r="AD14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE14" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF14" s="34">
+        <v>187.6</v>
+      </c>
+      <c r="AG14" s="34">
+        <v>39986.68</v>
+      </c>
+      <c r="AH14" s="34">
+        <v>163.80000000000001</v>
+      </c>
+      <c r="AI14" s="39">
+        <f>AF14/198</f>
+        <v>0.94747474747474747</v>
+      </c>
+      <c r="AJ14" s="41">
+        <v>7</v>
+      </c>
+      <c r="AL14" s="57">
+        <v>8</v>
+      </c>
+      <c r="AM14" s="52"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>100</v>
       </c>
@@ -10879,78 +11430,159 @@
       <c r="X15" t="s">
         <v>46</v>
       </c>
-      <c r="Y15" s="4">
+      <c r="Y15" s="22">
         <v>8</v>
       </c>
-      <c r="Z15" s="3">
+      <c r="Z15" s="34">
         <v>140.04</v>
       </c>
-      <c r="AA15" s="3">
+      <c r="AA15" s="34">
         <v>37154.92</v>
       </c>
-      <c r="AB15" s="3">
+      <c r="AB15" s="34">
         <v>220.4</v>
       </c>
-      <c r="AC15" s="29">
+      <c r="AC15" s="36">
         <f>Z15/148</f>
         <v>0.94621621621621621</v>
       </c>
       <c r="AD15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE15" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF15" s="34">
+        <v>140.04</v>
+      </c>
+      <c r="AG15" s="34">
+        <v>37154.92</v>
+      </c>
+      <c r="AH15" s="34">
+        <v>220.4</v>
+      </c>
+      <c r="AI15" s="39">
+        <f>AF15/148</f>
+        <v>0.94621621621621621</v>
+      </c>
+      <c r="AJ15" s="41">
+        <v>8</v>
+      </c>
+      <c r="AL15" s="57">
+        <v>9</v>
+      </c>
+      <c r="AM15" s="52"/>
+      <c r="AN15" s="51"/>
+      <c r="AO15" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="X16" t="s">
         <v>44</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Y16" s="15">
         <v>9</v>
       </c>
-      <c r="Z16" s="3">
+      <c r="Z16" s="34">
         <v>213.36</v>
       </c>
-      <c r="AA16" s="3">
+      <c r="AA16" s="34">
         <v>51289.88</v>
       </c>
-      <c r="AB16" s="3">
+      <c r="AB16" s="34">
         <v>80.2</v>
       </c>
-      <c r="AC16" s="29">
+      <c r="AC16" s="36">
         <f>Z16/247</f>
         <v>0.86380566801619441</v>
       </c>
       <c r="AD16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE16" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF16" s="34">
+        <v>213.36</v>
+      </c>
+      <c r="AG16" s="34">
+        <v>51289.88</v>
+      </c>
+      <c r="AH16" s="34">
+        <v>80.2</v>
+      </c>
+      <c r="AI16" s="39">
+        <f>AF16/247</f>
+        <v>0.86380566801619441</v>
+      </c>
+      <c r="AJ16" s="42">
+        <v>9</v>
+      </c>
+      <c r="AL16" s="57">
+        <v>10</v>
+      </c>
+      <c r="AM16" s="52"/>
+      <c r="AN16" s="51"/>
+      <c r="AO16" s="58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="X17" t="s">
         <v>45</v>
       </c>
-      <c r="Y17" s="4">
+      <c r="Y17" s="22">
         <v>10</v>
       </c>
-      <c r="Z17" s="4">
+      <c r="Z17" s="16">
         <v>201.36</v>
       </c>
-      <c r="AA17" s="4">
+      <c r="AA17" s="16">
         <v>72838.039999999994</v>
       </c>
-      <c r="AB17" s="3">
+      <c r="AB17" s="34">
         <v>66.56</v>
       </c>
-      <c r="AC17" s="29">
+      <c r="AC17" s="36">
         <f>Z17/247</f>
         <v>0.81522267206477739</v>
       </c>
       <c r="AD17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE17" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF17" s="16">
+        <v>201.36</v>
+      </c>
+      <c r="AG17" s="16">
+        <v>72838.039999999994</v>
+      </c>
+      <c r="AH17" s="34">
+        <v>66.56</v>
+      </c>
+      <c r="AI17" s="39">
+        <f>AF17/247</f>
+        <v>0.81522267206477739</v>
+      </c>
+      <c r="AJ17" s="41">
+        <v>10</v>
+      </c>
+      <c r="AL17" s="59">
+        <v>11</v>
+      </c>
+      <c r="AM17" s="60"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -10978,30 +11610,53 @@
       <c r="W18" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="X18" s="32" t="s">
+      <c r="X18" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="Y18" s="4">
+      <c r="Y18" s="23">
         <v>11</v>
       </c>
-      <c r="Z18" s="3">
+      <c r="Z18" s="37">
         <v>204.12</v>
       </c>
-      <c r="AA18" s="3">
+      <c r="AA18" s="37">
         <v>73388.08</v>
       </c>
-      <c r="AB18" s="3">
+      <c r="AB18" s="37">
         <v>74.239999999999995</v>
       </c>
-      <c r="AC18" s="29">
+      <c r="AC18" s="38">
         <f>Z18/247</f>
         <v>0.82639676113360327</v>
       </c>
       <c r="AD18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE18" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF18" s="37">
+        <v>204.12</v>
+      </c>
+      <c r="AG18" s="37">
+        <v>73388.08</v>
+      </c>
+      <c r="AH18" s="37">
+        <v>74.239999999999995</v>
+      </c>
+      <c r="AI18" s="44">
+        <f>AF18/247</f>
+        <v>0.82639676113360327</v>
+      </c>
+      <c r="AJ18" s="45">
+        <v>11</v>
+      </c>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="3"/>
+      <c r="AO18" s="3"/>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -11035,9 +11690,9 @@
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
       <c r="AB19" s="3"/>
-      <c r="AC19" s="29"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC19" s="28"/>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -11070,9 +11725,9 @@
       <c r="Y20" s="4"/>
       <c r="Z20" s="21"/>
       <c r="AA20" s="21"/>
-      <c r="AC20" s="31"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC20" s="29"/>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -11108,9 +11763,9 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="21"/>
       <c r="AA21" s="21"/>
-      <c r="AC21" s="31"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC21" s="29"/>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -11179,9 +11834,9 @@
       <c r="Y22" s="4"/>
       <c r="Z22" s="21"/>
       <c r="AA22" s="21"/>
-      <c r="AC22" s="31"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC22" s="29"/>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -11250,9 +11905,9 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="21"/>
       <c r="AA23" s="21"/>
-      <c r="AC23" s="31"/>
-    </row>
-    <row r="24" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC23" s="29"/>
+    </row>
+    <row r="24" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>10</v>
       </c>
@@ -11321,9 +11976,9 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="21"/>
       <c r="AA24" s="21"/>
-      <c r="AC24" s="31"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC24" s="29"/>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>15</v>
       </c>
@@ -11363,9 +12018,9 @@
       <c r="M25" s="4">
         <v>20.6</v>
       </c>
-      <c r="AC25" s="31"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC25" s="29"/>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -11406,7 +12061,7 @@
         <v>20.16</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>30</v>
       </c>
@@ -11447,7 +12102,7 @@
         <v>19.28</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>40</v>
       </c>
@@ -11488,17 +12143,17 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>

</xml_diff>